<commit_message>
Updated 01_sim.R Updated results xlsx files
</commit_message>
<xml_diff>
--- a/nico_type1_error.xlsx
+++ b/nico_type1_error.xlsx
@@ -436,40 +436,40 @@
         </is>
       </c>
       <c r="C2">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D2">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E2">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F2">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H2">
         <v>7</v>
       </c>
       <c r="I2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
         <v>9</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>11</v>
       </c>
-      <c r="L2">
-        <v>6</v>
-      </c>
-      <c r="M2">
-        <v>13</v>
-      </c>
       <c r="N2">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -479,19 +479,19 @@
         </is>
       </c>
       <c r="C3">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F3">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -500,19 +500,19 @@
         <v>9</v>
       </c>
       <c r="J3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K3">
         <v>6</v>
       </c>
       <c r="L3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N3">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -527,34 +527,34 @@
         </is>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4">
         <v>8</v>
-      </c>
-      <c r="F4">
-        <v>6</v>
-      </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
-      <c r="H4">
-        <v>4</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4">
-        <v>6</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
-      <c r="L4">
-        <v>5</v>
       </c>
       <c r="M4">
         <v>7</v>
@@ -575,37 +575,37 @@
         </is>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="J5">
         <v>4</v>
       </c>
-      <c r="I5">
-        <v>6</v>
-      </c>
-      <c r="J5">
-        <v>5</v>
-      </c>
       <c r="K5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N5">
         <v>5</v>
@@ -623,13 +623,13 @@
         </is>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E6">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F6">
         <v>6</v>
@@ -641,19 +641,19 @@
         <v>4</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L6">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M6">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="N6">
         <v>5</v>
@@ -671,19 +671,19 @@
         </is>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H7">
         <v>4</v>
@@ -692,19 +692,19 @@
         <v>6</v>
       </c>
       <c r="J7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L7">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M7">
         <v>8</v>
       </c>
       <c r="N7">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>